<commit_message>
Login for all users
</commit_message>
<xml_diff>
--- a/Sprint 3 Backlog.xlsx
+++ b/Sprint 3 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karim_i45ca1v\707\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5947C76-90B8-4826-8108-3230819F6B4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB7A762-F6E8-4EAF-93FE-30DE9A04CA57}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -380,7 +380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,9 +479,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -488,14 +491,17 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,21 +843,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BWM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="195.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="195.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -872,11 +878,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1963" s="10" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:1963" s="9" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="18">
         <v>1.1000000000000001</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -2851,8 +2857,8 @@
       <c r="BWL2"/>
       <c r="BWM2"/>
     </row>
-    <row r="3" spans="1:1963" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:1963" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14"/>
       <c r="B3" s="4" t="s">
         <v>73</v>
       </c>
@@ -2872,8 +2878,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+    <row r="4" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>74</v>
       </c>
@@ -2893,8 +2899,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+    <row r="5" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
@@ -2914,8 +2920,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+    <row r="6" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
         <v>76</v>
       </c>
@@ -2935,8 +2941,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+    <row r="7" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="14"/>
       <c r="B7" s="4" t="s">
         <v>77</v>
       </c>
@@ -2956,8 +2962,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
       <c r="B8" s="4" t="s">
         <v>78</v>
       </c>
@@ -2977,8 +2983,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:1963" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+    <row r="9" spans="1:1963" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14"/>
       <c r="B9" s="4" t="s">
         <v>79</v>
       </c>
@@ -2998,8 +3004,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+    <row r="10" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="14"/>
       <c r="B10" s="5" t="s">
         <v>80</v>
       </c>
@@ -3019,8 +3025,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
@@ -3040,8 +3046,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+    <row r="12" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
@@ -3061,9 +3067,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="11">
+    <row r="13" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
+      <c r="B13" s="10">
         <v>1.1200000000000001</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -5038,9 +5044,9 @@
       <c r="BWL13"/>
       <c r="BWM13"/>
     </row>
-    <row r="14" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="11">
+    <row r="14" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="10">
         <v>1.1299999999999999</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -7015,9 +7021,9 @@
       <c r="BWL14"/>
       <c r="BWM14"/>
     </row>
-    <row r="15" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="11">
+    <row r="15" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="10">
         <v>1.1399999999999999</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -8992,9 +8998,9 @@
       <c r="BWL15"/>
       <c r="BWM15"/>
     </row>
-    <row r="16" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="11">
+    <row r="16" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="10">
         <v>1.1499999999999999</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -10969,11 +10975,11 @@
       <c r="BWL16"/>
       <c r="BWM16"/>
     </row>
-    <row r="17" spans="1:1963" s="12" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:1963" s="11" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="18">
         <v>2.1</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -12948,9 +12954,9 @@
       <c r="BWL17"/>
       <c r="BWM17"/>
     </row>
-    <row r="18" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>2.2000000000000002</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -14925,11 +14931,11 @@
       <c r="BWL18"/>
       <c r="BWM18"/>
     </row>
-    <row r="19" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="18">
         <v>3.1</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -16904,7 +16910,7 @@
       <c r="BWL19"/>
       <c r="BWM19"/>
     </row>
-    <row r="20" spans="1:1963" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1963" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17"/>
       <c r="B20" s="4" t="s">
         <v>3</v>
@@ -16925,9 +16931,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="17"/>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -16946,9 +16952,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="17"/>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -16967,12 +16973,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="17"/>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D23">
@@ -16988,7 +16994,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="17"/>
       <c r="B24" s="4" t="s">
         <v>7</v>
@@ -17009,7 +17015,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="17"/>
       <c r="B25" s="4" t="s">
         <v>8</v>
@@ -17030,7 +17036,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="17"/>
       <c r="B26" s="4" t="s">
         <v>10</v>
@@ -17051,7 +17057,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="17"/>
       <c r="B27" s="4" t="s">
         <v>11</v>
@@ -17072,7 +17078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="17"/>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -17093,7 +17099,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
       <c r="B29" s="4" t="s">
         <v>13</v>
@@ -17114,7 +17120,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="17"/>
       <c r="B30" s="4" t="s">
         <v>82</v>
@@ -17135,7 +17141,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="17"/>
       <c r="B31" s="4" t="s">
         <v>83</v>
@@ -17156,7 +17162,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>45</v>
       </c>
@@ -17179,7 +17185,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="17"/>
       <c r="B33" s="4" t="s">
         <v>34</v>
@@ -17200,7 +17206,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="17"/>
       <c r="B34" s="4" t="s">
         <v>35</v>
@@ -17221,7 +17227,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="17"/>
       <c r="B35" s="4" t="s">
         <v>36</v>
@@ -17242,9 +17248,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="17"/>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -17263,9 +17269,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17"/>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -17284,7 +17290,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="17"/>
       <c r="B38" s="4" t="s">
         <v>39</v>
@@ -17305,7 +17311,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="17"/>
       <c r="B39" s="4" t="s">
         <v>40</v>
@@ -17326,7 +17332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="17"/>
       <c r="B40" s="4" t="s">
         <v>41</v>
@@ -17347,7 +17353,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="17"/>
       <c r="B41" s="4" t="s">
         <v>42</v>
@@ -17368,9 +17374,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="17"/>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -17389,9 +17395,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="17"/>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -17410,22 +17416,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final today's Kariman & Peter
</commit_message>
<xml_diff>
--- a/Sprint 3 Backlog.xlsx
+++ b/Sprint 3 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karim_i45ca1v\707\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5947C76-90B8-4826-8108-3230819F6B4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB7A762-F6E8-4EAF-93FE-30DE9A04CA57}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -380,7 +380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,9 +479,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -488,14 +491,17 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,21 +843,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BWM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="195.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="195.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" customWidth="1"/>
+    <col min="5" max="5" width="8.08984375" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -872,11 +878,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1963" s="10" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:1963" s="9" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="18">
         <v>1.1000000000000001</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -2851,8 +2857,8 @@
       <c r="BWL2"/>
       <c r="BWM2"/>
     </row>
-    <row r="3" spans="1:1963" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:1963" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14"/>
       <c r="B3" s="4" t="s">
         <v>73</v>
       </c>
@@ -2872,8 +2878,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+    <row r="4" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>74</v>
       </c>
@@ -2893,8 +2899,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+    <row r="5" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="14"/>
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
@@ -2914,8 +2920,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+    <row r="6" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
         <v>76</v>
       </c>
@@ -2935,8 +2941,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+    <row r="7" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="14"/>
       <c r="B7" s="4" t="s">
         <v>77</v>
       </c>
@@ -2956,8 +2962,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
       <c r="B8" s="4" t="s">
         <v>78</v>
       </c>
@@ -2977,8 +2983,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:1963" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+    <row r="9" spans="1:1963" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14"/>
       <c r="B9" s="4" t="s">
         <v>79</v>
       </c>
@@ -2998,8 +3004,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+    <row r="10" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="14"/>
       <c r="B10" s="5" t="s">
         <v>80</v>
       </c>
@@ -3019,8 +3025,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
@@ -3040,8 +3046,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+    <row r="12" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
@@ -3061,9 +3067,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="11">
+    <row r="13" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
+      <c r="B13" s="10">
         <v>1.1200000000000001</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -5038,9 +5044,9 @@
       <c r="BWL13"/>
       <c r="BWM13"/>
     </row>
-    <row r="14" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="11">
+    <row r="14" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="10">
         <v>1.1299999999999999</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -7015,9 +7021,9 @@
       <c r="BWL14"/>
       <c r="BWM14"/>
     </row>
-    <row r="15" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="11">
+    <row r="15" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="10">
         <v>1.1399999999999999</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -8992,9 +8998,9 @@
       <c r="BWL15"/>
       <c r="BWM15"/>
     </row>
-    <row r="16" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="11">
+    <row r="16" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="10">
         <v>1.1499999999999999</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -10969,11 +10975,11 @@
       <c r="BWL16"/>
       <c r="BWM16"/>
     </row>
-    <row r="17" spans="1:1963" s="12" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:1963" s="11" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="18">
         <v>2.1</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -12948,9 +12954,9 @@
       <c r="BWL17"/>
       <c r="BWM17"/>
     </row>
-    <row r="18" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>2.2000000000000002</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -14925,11 +14931,11 @@
       <c r="BWL18"/>
       <c r="BWM18"/>
     </row>
-    <row r="19" spans="1:1963" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1963" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="18">
         <v>3.1</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -16904,7 +16910,7 @@
       <c r="BWL19"/>
       <c r="BWM19"/>
     </row>
-    <row r="20" spans="1:1963" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1963" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17"/>
       <c r="B20" s="4" t="s">
         <v>3</v>
@@ -16925,9 +16931,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="17"/>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -16946,9 +16952,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="17"/>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -16967,12 +16973,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="17"/>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D23">
@@ -16988,7 +16994,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="17"/>
       <c r="B24" s="4" t="s">
         <v>7</v>
@@ -17009,7 +17015,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="17"/>
       <c r="B25" s="4" t="s">
         <v>8</v>
@@ -17030,7 +17036,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="17"/>
       <c r="B26" s="4" t="s">
         <v>10</v>
@@ -17051,7 +17057,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="17"/>
       <c r="B27" s="4" t="s">
         <v>11</v>
@@ -17072,7 +17078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="17"/>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -17093,7 +17099,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
       <c r="B29" s="4" t="s">
         <v>13</v>
@@ -17114,7 +17120,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="17"/>
       <c r="B30" s="4" t="s">
         <v>82</v>
@@ -17135,7 +17141,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="17"/>
       <c r="B31" s="4" t="s">
         <v>83</v>
@@ -17156,7 +17162,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1963" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>45</v>
       </c>
@@ -17179,7 +17185,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="17"/>
       <c r="B33" s="4" t="s">
         <v>34</v>
@@ -17200,7 +17206,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="17"/>
       <c r="B34" s="4" t="s">
         <v>35</v>
@@ -17221,7 +17227,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="17"/>
       <c r="B35" s="4" t="s">
         <v>36</v>
@@ -17242,9 +17248,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="17"/>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -17263,9 +17269,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17"/>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -17284,7 +17290,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="17"/>
       <c r="B38" s="4" t="s">
         <v>39</v>
@@ -17305,7 +17311,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="17"/>
       <c r="B39" s="4" t="s">
         <v>40</v>
@@ -17326,7 +17332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="17"/>
       <c r="B40" s="4" t="s">
         <v>41</v>
@@ -17347,7 +17353,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="17"/>
       <c r="B41" s="4" t="s">
         <v>42</v>
@@ -17368,9 +17374,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="17"/>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -17389,9 +17395,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="17"/>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -17410,22 +17416,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="8"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All stories are done
</commit_message>
<xml_diff>
--- a/Sprint 3 Backlog.xlsx
+++ b/Sprint 3 Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Desktop\707\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5220EB61-9620-46A0-B1EB-F925C8436AA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6DE7EA-D392-4CBF-A496-6A9C451F7B12}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="92">
   <si>
     <t>User story</t>
   </si>
@@ -466,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,18 +477,12 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -858,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BWM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,24 +877,24 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1963" s="8" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:1963" s="7" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D2">
@@ -2873,11 +2867,11 @@
       <c r="BWM2"/>
     </row>
     <row r="3" spans="1:1963" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D3">
@@ -2894,11 +2888,11 @@
       </c>
     </row>
     <row r="4" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D4">
@@ -2915,11 +2909,11 @@
       </c>
     </row>
     <row r="5" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D5">
@@ -2936,11 +2930,11 @@
       </c>
     </row>
     <row r="6" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D6">
@@ -2957,11 +2951,11 @@
       </c>
     </row>
     <row r="7" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D7">
@@ -2978,11 +2972,11 @@
       </c>
     </row>
     <row r="8" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D8">
@@ -2999,11 +2993,11 @@
       </c>
     </row>
     <row r="9" spans="1:1963" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D9">
@@ -3020,11 +3014,11 @@
       </c>
     </row>
     <row r="10" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D10">
@@ -3041,11 +3035,11 @@
       </c>
     </row>
     <row r="11" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D11">
@@ -3062,11 +3056,11 @@
       </c>
     </row>
     <row r="12" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D12">
@@ -3082,12 +3076,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:1963" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="12">
+    <row r="13" spans="1:1963" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="10">
         <v>1.1200000000000001</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D13">
@@ -5059,12 +5053,12 @@
       <c r="BWL13"/>
       <c r="BWM13"/>
     </row>
-    <row r="14" spans="1:1963" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
-      <c r="B14" s="12">
+    <row r="14" spans="1:1963" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="10">
         <v>1.1299999999999999</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D14">
@@ -7036,12 +7030,12 @@
       <c r="BWL14"/>
       <c r="BWM14"/>
     </row>
-    <row r="15" spans="1:1963" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="12">
+    <row r="15" spans="1:1963" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="10">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D15">
@@ -9013,12 +9007,12 @@
       <c r="BWL15"/>
       <c r="BWM15"/>
     </row>
-    <row r="16" spans="1:1963" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="9">
+    <row r="16" spans="1:1963" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="10">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D16">
@@ -10990,14 +10984,14 @@
       <c r="BWL16"/>
       <c r="BWM16"/>
     </row>
-    <row r="17" spans="1:1963" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:1963" s="8" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="10">
         <v>2.1</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D17">
@@ -12969,12 +12963,12 @@
       <c r="BWL17"/>
       <c r="BWM17"/>
     </row>
-    <row r="18" spans="1:1963" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="9">
+    <row r="18" spans="1:1963" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="10">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D18">
@@ -14946,14 +14940,14 @@
       <c r="BWL18"/>
       <c r="BWM18"/>
     </row>
-    <row r="19" spans="1:1963" s="10" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:1963" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="10">
         <v>3.1</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D19">
@@ -16926,11 +16920,11 @@
       <c r="BWM19"/>
     </row>
     <row r="20" spans="1:1963" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="18"/>
+      <c r="B20" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D20">
@@ -16947,11 +16941,11 @@
       </c>
     </row>
     <row r="21" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="18"/>
+      <c r="B21" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D21">
@@ -16968,11 +16962,11 @@
       </c>
     </row>
     <row r="22" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="18"/>
+      <c r="B22" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>90</v>
       </c>
       <c r="D22">
@@ -16989,11 +16983,11 @@
       </c>
     </row>
     <row r="23" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D23">
@@ -17010,11 +17004,11 @@
       </c>
     </row>
     <row r="24" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="18"/>
+      <c r="B24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D24">
@@ -17031,11 +17025,11 @@
       </c>
     </row>
     <row r="25" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25">
@@ -17052,11 +17046,11 @@
       </c>
     </row>
     <row r="26" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="18"/>
+      <c r="B26" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D26">
@@ -17073,11 +17067,11 @@
       </c>
     </row>
     <row r="27" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="13" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D27">
@@ -17094,11 +17088,11 @@
       </c>
     </row>
     <row r="28" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="13" t="s">
+      <c r="A28" s="18"/>
+      <c r="B28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D28">
@@ -17115,11 +17109,11 @@
       </c>
     </row>
     <row r="29" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="13" t="s">
+      <c r="A29" s="18"/>
+      <c r="B29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D29">
@@ -17136,11 +17130,11 @@
       </c>
     </row>
     <row r="30" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="13" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D30">
@@ -17157,11 +17151,11 @@
       </c>
     </row>
     <row r="31" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="18"/>
+      <c r="B31" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D31">
@@ -17178,13 +17172,13 @@
       </c>
     </row>
     <row r="32" spans="1:1963" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D32">
@@ -17201,11 +17195,11 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
-      <c r="B33" s="13" t="s">
+      <c r="A33" s="18"/>
+      <c r="B33" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D33">
@@ -17222,11 +17216,11 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="20"/>
-      <c r="B34" s="13" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D34">
@@ -17243,11 +17237,11 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="13" t="s">
+      <c r="A35" s="18"/>
+      <c r="B35" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D35">
@@ -17264,11 +17258,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="20"/>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="18"/>
+      <c r="B36" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D36">
@@ -17285,11 +17279,11 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="20"/>
-      <c r="B37" s="15" t="s">
+      <c r="A37" s="18"/>
+      <c r="B37" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D37">
@@ -17306,11 +17300,11 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="20"/>
-      <c r="B38" s="13" t="s">
+      <c r="A38" s="18"/>
+      <c r="B38" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D38">
@@ -17327,11 +17321,11 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="20"/>
-      <c r="B39" s="13" t="s">
+      <c r="A39" s="18"/>
+      <c r="B39" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D39">
@@ -17348,11 +17342,11 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="20"/>
-      <c r="B40" s="13" t="s">
+      <c r="A40" s="18"/>
+      <c r="B40" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D40">
@@ -17369,11 +17363,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="20"/>
-      <c r="B41" s="13" t="s">
+      <c r="A41" s="18"/>
+      <c r="B41" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D41">
@@ -17390,11 +17384,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="20"/>
-      <c r="B42" s="16" t="s">
+      <c r="A42" s="18"/>
+      <c r="B42" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D42" t="s">
@@ -17411,11 +17405,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-      <c r="B43" s="15" t="s">
+      <c r="A43" s="18"/>
+      <c r="B43" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D43">
@@ -17432,22 +17426,22 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="6"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
+      <c r="A46" s="6"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
+      <c r="A48" s="6"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
+      <c r="A49" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>